<commit_message>
added updated python scripts
</commit_message>
<xml_diff>
--- a/datalogging/power consumption/energest/converted2_4-merged.xlsx
+++ b/datalogging/power consumption/energest/converted2_4-merged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Univ\SensorManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EDAFB4-DC92-4E2B-9655-0BF6471E556A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67645C8-B5CC-42ED-B38A-A1A69A701A3C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="run1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="26">
   <si>
     <t>packet</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>individual packet:</t>
+  </si>
+  <si>
+    <t>x voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mW/h: </t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -582,8 +591,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -942,13 +952,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L332"/>
+  <dimension ref="A1:O338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
-      <selection activeCell="N327" sqref="N327"/>
+    <sheetView topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="H309" sqref="H309:L312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -959,21 +974,21 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -13010,7 +13025,7 @@
         <v>298.46636962890625</v>
       </c>
     </row>
-    <row r="306" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="306" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D306" t="s">
         <v>9</v>
       </c>
@@ -13019,7 +13034,7 @@
         <v>295.73062133789063</v>
       </c>
     </row>
-    <row r="308" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="308" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D308" t="s">
         <v>10</v>
       </c>
@@ -13039,83 +13054,83 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="309" spans="4:15" x14ac:dyDescent="0.3">
       <c r="H309">
-        <f>20*10^-6</f>
-        <v>1.9999999999999998E-5</v>
+        <f>20*10^-3</f>
+        <v>0.02</v>
       </c>
       <c r="K309">
-        <f>24*10^-6</f>
-        <v>2.4000000000000001E-5</v>
+        <f>24*10^-3</f>
+        <v>2.4E-2</v>
       </c>
       <c r="L309">
-        <f>20*10^-6</f>
-        <v>1.9999999999999998E-5</v>
-      </c>
-    </row>
-    <row r="310" spans="4:12" x14ac:dyDescent="0.3">
+        <f>20*10^-3</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="310" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E310" t="s">
         <v>16</v>
       </c>
       <c r="I310">
-        <f>0.6*10^-6</f>
-        <v>5.9999999999999997E-7</v>
-      </c>
-    </row>
-    <row r="311" spans="4:12" x14ac:dyDescent="0.3">
+        <f>0.6*10^-3</f>
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="311" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E311" t="s">
         <v>17</v>
       </c>
       <c r="I311">
-        <f>1.3*10^-9</f>
-        <v>1.3000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="312" spans="4:12" x14ac:dyDescent="0.3">
+        <f>1.3*10^-6</f>
+        <v>1.3E-6</v>
+      </c>
+    </row>
+    <row r="312" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E312" t="s">
         <v>18</v>
       </c>
       <c r="I312">
-        <f>0.4*10^-9</f>
-        <v>4.0000000000000007E-10</v>
-      </c>
-    </row>
-    <row r="314" spans="4:12" x14ac:dyDescent="0.3">
+        <f>0.4*10^-6</f>
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="314" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D314" t="s">
         <v>19</v>
       </c>
       <c r="H314">
         <f>H303*H309</f>
-        <v>7.960021972656249E-5</v>
+        <v>7.9600219726562504E-2</v>
       </c>
       <c r="K314">
         <f>K303*K309</f>
-        <v>1.2832763671875E-5</v>
+        <v>1.2832763671875001E-2</v>
       </c>
       <c r="L314">
         <f>L303*L309</f>
-        <v>5.9693273925781245E-3</v>
-      </c>
-    </row>
-    <row r="315" spans="4:12" x14ac:dyDescent="0.3">
+        <v>5.9693273925781254</v>
+      </c>
+    </row>
+    <row r="315" spans="4:15" x14ac:dyDescent="0.3">
       <c r="I315">
         <f>I306*I310</f>
-        <v>1.7743837280273438E-4</v>
-      </c>
-    </row>
-    <row r="316" spans="4:12" x14ac:dyDescent="0.3">
+        <v>0.17743837280273436</v>
+      </c>
+    </row>
+    <row r="316" spans="4:15" x14ac:dyDescent="0.3">
       <c r="I316">
         <f>I306*I311</f>
-        <v>3.8444980773925782E-7</v>
-      </c>
-    </row>
-    <row r="317" spans="4:12" x14ac:dyDescent="0.3">
+        <v>3.8444980773925784E-4</v>
+      </c>
+    </row>
+    <row r="317" spans="4:15" x14ac:dyDescent="0.3">
       <c r="I317">
         <f>I306*I312</f>
-        <v>1.1829224853515627E-7</v>
-      </c>
-    </row>
-    <row r="320" spans="4:12" x14ac:dyDescent="0.3">
+        <v>1.1829224853515624E-4</v>
+      </c>
+    </row>
+    <row r="320" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D320" t="s">
         <v>20</v>
       </c>
@@ -13124,37 +13139,82 @@
       </c>
       <c r="G320">
         <f>H309+K309+L309</f>
-        <v>6.3999999999999997E-5</v>
-      </c>
-    </row>
-    <row r="321" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="I320" t="s">
+        <v>23</v>
+      </c>
+      <c r="J320">
+        <v>3.7</v>
+      </c>
+      <c r="K320">
+        <f>J320*G320</f>
+        <v>0.23680000000000001</v>
+      </c>
+      <c r="M320" t="s">
+        <v>24</v>
+      </c>
+      <c r="N320">
+        <f>(K320/12) * 1000</f>
+        <v>19.733333333333334</v>
+      </c>
+      <c r="O320">
+        <f>(K320*1000)/12</f>
+        <v>19.733333333333334</v>
+      </c>
+    </row>
+    <row r="321" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E321" t="s">
         <v>16</v>
       </c>
       <c r="G321">
         <f>G320+I310</f>
-        <v>6.4599999999999998E-5</v>
-      </c>
-    </row>
-    <row r="322" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4600000000000005E-2</v>
+      </c>
+      <c r="K321">
+        <f>G321*J320</f>
+        <v>0.23902000000000004</v>
+      </c>
+      <c r="N321">
+        <f>(K321/12) * 1000</f>
+        <v>19.918333333333337</v>
+      </c>
+    </row>
+    <row r="322" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E322" t="s">
         <v>17</v>
       </c>
       <c r="G322">
         <f>G320+I311</f>
-        <v>6.4001299999999993E-5</v>
-      </c>
-    </row>
-    <row r="323" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4001299999999997E-2</v>
+      </c>
+      <c r="K322">
+        <f>G322*J320</f>
+        <v>0.23680481</v>
+      </c>
+      <c r="N322">
+        <f>(K322/12) * 1000</f>
+        <v>19.733734166666665</v>
+      </c>
+    </row>
+    <row r="323" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E323" t="s">
         <v>18</v>
       </c>
       <c r="G323">
         <f>G320+I312</f>
-        <v>6.4000399999999998E-5</v>
-      </c>
-    </row>
-    <row r="327" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4000399999999999E-2</v>
+      </c>
+      <c r="K323">
+        <f>G323*J320</f>
+        <v>0.23680148000000001</v>
+      </c>
+      <c r="N323">
+        <f>(K323/12) * 1000</f>
+        <v>19.733456666666665</v>
+      </c>
+    </row>
+    <row r="327" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D327" t="s">
         <v>22</v>
       </c>
@@ -13175,48 +13235,127 @@
         <v>0.99822998046875</v>
       </c>
     </row>
-    <row r="329" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="329" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D329" t="s">
         <v>19</v>
       </c>
       <c r="H329">
         <f>H309*H314</f>
-        <v>1.5920043945312497E-9</v>
+        <v>1.5920043945312501E-3</v>
       </c>
       <c r="K329">
         <f>K327*K309</f>
-        <v>4.248046875E-8</v>
+        <v>4.2480468750000004E-5</v>
       </c>
       <c r="L329">
         <f>L309*L327</f>
-        <v>1.9964599609374997E-5</v>
-      </c>
-    </row>
-    <row r="330" spans="4:12" x14ac:dyDescent="0.3">
+        <v>1.9964599609375001E-2</v>
+      </c>
+      <c r="N329" t="s">
+        <v>23</v>
+      </c>
+      <c r="O329">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="330" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E330" t="s">
         <v>16</v>
       </c>
       <c r="I330">
         <f>I310*I327</f>
-        <v>5.92401123046875E-7</v>
-      </c>
-    </row>
-    <row r="331" spans="4:12" x14ac:dyDescent="0.3">
+        <v>5.9240112304687498E-4</v>
+      </c>
+      <c r="O330" s="1">
+        <f>I330*O329</f>
+        <v>2.1918841552734376E-3</v>
+      </c>
+    </row>
+    <row r="331" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E331" t="s">
         <v>17</v>
       </c>
       <c r="I331">
         <f>I316*I327</f>
-        <v>3.7958082976648584E-7</v>
-      </c>
-    </row>
-    <row r="332" spans="4:12" x14ac:dyDescent="0.3">
+        <v>3.7958082976648585E-4</v>
+      </c>
+      <c r="O331" s="1">
+        <f>I331*O329</f>
+        <v>1.4044490701359978E-3</v>
+      </c>
+    </row>
+    <row r="332" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E332" t="s">
         <v>18</v>
       </c>
       <c r="I332">
         <f>I312*I327</f>
-        <v>3.9493408203125007E-10</v>
+        <v>3.9493408203125E-7</v>
+      </c>
+      <c r="O332" s="1">
+        <f>I332*O329</f>
+        <v>1.4612561035156252E-6</v>
+      </c>
+    </row>
+    <row r="335" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D335" t="s">
+        <v>20</v>
+      </c>
+      <c r="E335" t="s">
+        <v>21</v>
+      </c>
+      <c r="G335">
+        <f>H329+K329+L329</f>
+        <v>2.1599084472656252E-2</v>
+      </c>
+      <c r="I335" t="s">
+        <v>23</v>
+      </c>
+      <c r="J335">
+        <v>3.7</v>
+      </c>
+      <c r="K335">
+        <f>G335*J335</f>
+        <v>7.9916612548828134E-2</v>
+      </c>
+    </row>
+    <row r="336" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="E336" t="s">
+        <v>16</v>
+      </c>
+      <c r="G336">
+        <f>G335+I330</f>
+        <v>2.2191485595703126E-2</v>
+      </c>
+      <c r="K336">
+        <f>G336*J335</f>
+        <v>8.2108496704101572E-2</v>
+      </c>
+    </row>
+    <row r="337" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E337" t="s">
+        <v>17</v>
+      </c>
+      <c r="G337">
+        <f>G335+I331</f>
+        <v>2.1978665302422738E-2</v>
+      </c>
+      <c r="K337">
+        <f>G337*J335</f>
+        <v>8.132106161896413E-2</v>
+      </c>
+    </row>
+    <row r="338" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E338" t="s">
+        <v>18</v>
+      </c>
+      <c r="G338">
+        <f>H329+I332</f>
+        <v>1.5923993286132813E-3</v>
+      </c>
+      <c r="K338">
+        <f>G338*J335</f>
+        <v>5.891877515869141E-3</v>
       </c>
     </row>
   </sheetData>
@@ -13230,10 +13369,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L332"/>
+  <dimension ref="A1:O338"/>
   <sheetViews>
-    <sheetView topLeftCell="A308" workbookViewId="0">
-      <selection activeCell="D327" sqref="D327:L332"/>
+    <sheetView topLeftCell="A299" workbookViewId="0">
+      <selection activeCell="H309" sqref="H309:L312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13247,21 +13386,21 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -25298,7 +25437,7 @@
         <v>298.4718017578125</v>
       </c>
     </row>
-    <row r="306" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="306" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D306" t="s">
         <v>9</v>
       </c>
@@ -25307,7 +25446,7 @@
         <v>295.633544921875</v>
       </c>
     </row>
-    <row r="308" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="308" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D308" t="s">
         <v>10</v>
       </c>
@@ -25327,83 +25466,83 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="309" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H309">
-        <f>20*10^-6</f>
-        <v>1.9999999999999998E-5</v>
+        <f>20*10^-3</f>
+        <v>0.02</v>
       </c>
       <c r="K309">
-        <f>24*10^-6</f>
-        <v>2.4000000000000001E-5</v>
+        <f>24*10^-3</f>
+        <v>2.4E-2</v>
       </c>
       <c r="L309">
-        <f>20*10^-6</f>
-        <v>1.9999999999999998E-5</v>
-      </c>
-    </row>
-    <row r="310" spans="4:12" x14ac:dyDescent="0.3">
+        <f>20*10^-3</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="310" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E310" t="s">
         <v>16</v>
       </c>
       <c r="I310">
-        <f>0.6*10^-6</f>
-        <v>5.9999999999999997E-7</v>
-      </c>
-    </row>
-    <row r="311" spans="4:12" x14ac:dyDescent="0.3">
+        <f>0.6*10^-3</f>
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="311" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E311" t="s">
         <v>17</v>
       </c>
       <c r="I311">
-        <f>1.3*10^-9</f>
-        <v>1.3000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="312" spans="4:12" x14ac:dyDescent="0.3">
+        <f>1.3*10^-6</f>
+        <v>1.3E-6</v>
+      </c>
+    </row>
+    <row r="312" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E312" t="s">
         <v>18</v>
       </c>
       <c r="I312">
-        <f>0.4*10^-9</f>
-        <v>4.0000000000000007E-10</v>
-      </c>
-    </row>
-    <row r="314" spans="4:12" x14ac:dyDescent="0.3">
+        <f>0.4*10^-6</f>
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="314" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D314" t="s">
         <v>19</v>
       </c>
       <c r="H314">
         <f>H303*H309</f>
-        <v>8.1553955078124995E-5</v>
+        <v>8.1553955078125004E-2</v>
       </c>
       <c r="K314">
         <f>K303*K309</f>
-        <v>1.2720703125000001E-5</v>
+        <v>1.2720703125E-2</v>
       </c>
       <c r="L314">
         <f>L303*L309</f>
-        <v>5.9694360351562493E-3</v>
-      </c>
-    </row>
-    <row r="315" spans="4:12" x14ac:dyDescent="0.3">
+        <v>5.9694360351562503</v>
+      </c>
+    </row>
+    <row r="315" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I315">
         <f>I306*I310</f>
-        <v>1.77380126953125E-4</v>
-      </c>
-    </row>
-    <row r="316" spans="4:12" x14ac:dyDescent="0.3">
+        <v>0.17738012695312499</v>
+      </c>
+    </row>
+    <row r="316" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I316">
         <f>I306*I311</f>
-        <v>3.8432360839843752E-7</v>
-      </c>
-    </row>
-    <row r="317" spans="4:12" x14ac:dyDescent="0.3">
+        <v>3.8432360839843753E-4</v>
+      </c>
+    </row>
+    <row r="317" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I317">
         <f>I306*I312</f>
-        <v>1.1825341796875002E-7</v>
-      </c>
-    </row>
-    <row r="320" spans="4:12" x14ac:dyDescent="0.3">
+        <v>1.1825341796874999E-4</v>
+      </c>
+    </row>
+    <row r="320" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D320" t="s">
         <v>20</v>
       </c>
@@ -25412,37 +25551,78 @@
       </c>
       <c r="G320">
         <f>H309+K309+L309</f>
-        <v>6.3999999999999997E-5</v>
-      </c>
-    </row>
-    <row r="321" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="I320" t="s">
+        <v>23</v>
+      </c>
+      <c r="J320">
+        <v>3.7</v>
+      </c>
+      <c r="K320">
+        <f>J320*G320</f>
+        <v>0.23680000000000001</v>
+      </c>
+      <c r="M320" t="s">
+        <v>24</v>
+      </c>
+      <c r="N320">
+        <f>(K320/12) * 1000</f>
+        <v>19.733333333333334</v>
+      </c>
+    </row>
+    <row r="321" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E321" t="s">
         <v>16</v>
       </c>
       <c r="G321">
         <f>G320+I310</f>
-        <v>6.4599999999999998E-5</v>
-      </c>
-    </row>
-    <row r="322" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4600000000000005E-2</v>
+      </c>
+      <c r="K321">
+        <f>G321*J320</f>
+        <v>0.23902000000000004</v>
+      </c>
+      <c r="N321">
+        <f>(K321/12) * 1000</f>
+        <v>19.918333333333337</v>
+      </c>
+    </row>
+    <row r="322" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E322" t="s">
         <v>17</v>
       </c>
       <c r="G322">
         <f>G320+I311</f>
-        <v>6.4001299999999993E-5</v>
-      </c>
-    </row>
-    <row r="323" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4001299999999997E-2</v>
+      </c>
+      <c r="K322">
+        <f>G322*J320</f>
+        <v>0.23680481</v>
+      </c>
+      <c r="N322">
+        <f>(K322/12) * 1000</f>
+        <v>19.733734166666665</v>
+      </c>
+    </row>
+    <row r="323" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E323" t="s">
         <v>18</v>
       </c>
       <c r="G323">
         <f>G320+I312</f>
-        <v>6.4000399999999998E-5</v>
-      </c>
-    </row>
-    <row r="327" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4000399999999999E-2</v>
+      </c>
+      <c r="K323">
+        <f>G323*J320</f>
+        <v>0.23680148000000001</v>
+      </c>
+      <c r="N323">
+        <f>(K323/12) * 1000</f>
+        <v>19.733456666666665</v>
+      </c>
+    </row>
+    <row r="327" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D327" t="s">
         <v>22</v>
       </c>
@@ -25463,48 +25643,127 @@
         <v>0.99822998046875</v>
       </c>
     </row>
-    <row r="329" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="329" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D329" t="s">
         <v>19</v>
       </c>
       <c r="H329">
         <f>H309*H314</f>
-        <v>1.6310791015624998E-9</v>
+        <v>1.6310791015625001E-3</v>
       </c>
       <c r="K329">
         <f>K327*K309</f>
-        <v>4.1748046875000002E-8</v>
+        <v>4.1748046875000003E-5</v>
       </c>
       <c r="L329">
         <f>L309*L327</f>
-        <v>1.9964599609374997E-5</v>
-      </c>
-    </row>
-    <row r="330" spans="4:12" x14ac:dyDescent="0.3">
+        <v>1.9964599609375001E-2</v>
+      </c>
+      <c r="N329" t="s">
+        <v>23</v>
+      </c>
+      <c r="O329">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="330" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E330" t="s">
         <v>16</v>
       </c>
       <c r="I330">
         <f>I310*I327</f>
-        <v>5.9245605468749999E-7</v>
-      </c>
-    </row>
-    <row r="331" spans="4:12" x14ac:dyDescent="0.3">
+        <v>5.9245605468749997E-4</v>
+      </c>
+      <c r="O330" s="1">
+        <f>I330*O329</f>
+        <v>2.19208740234375E-3</v>
+      </c>
+    </row>
+    <row r="331" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E331" t="s">
         <v>17</v>
       </c>
       <c r="I331">
         <f>I316*I327</f>
-        <v>3.7949141459167005E-7</v>
-      </c>
-    </row>
-    <row r="332" spans="4:12" x14ac:dyDescent="0.3">
+        <v>3.7949141459167005E-4</v>
+      </c>
+      <c r="O331" s="1">
+        <f>I331*O329</f>
+        <v>1.4041182339891794E-3</v>
+      </c>
+    </row>
+    <row r="332" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E332" t="s">
         <v>18</v>
       </c>
       <c r="I332">
         <f>I312*I327</f>
-        <v>3.9497070312500005E-10</v>
+        <v>3.9497070312499999E-7</v>
+      </c>
+      <c r="O332" s="1">
+        <f>I332*O329</f>
+        <v>1.4613916015625E-6</v>
+      </c>
+    </row>
+    <row r="335" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D335" t="s">
+        <v>20</v>
+      </c>
+      <c r="E335" t="s">
+        <v>21</v>
+      </c>
+      <c r="G335">
+        <f>H329+K329+L329</f>
+        <v>2.1637426757812502E-2</v>
+      </c>
+      <c r="I335" t="s">
+        <v>23</v>
+      </c>
+      <c r="J335">
+        <v>3.7</v>
+      </c>
+      <c r="K335">
+        <f>G335*J335</f>
+        <v>8.0058479003906266E-2</v>
+      </c>
+    </row>
+    <row r="336" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="E336" t="s">
+        <v>16</v>
+      </c>
+      <c r="G336">
+        <f>G335+I330</f>
+        <v>2.2229882812500001E-2</v>
+      </c>
+      <c r="K336">
+        <f>G336*J335</f>
+        <v>8.2250566406250003E-2</v>
+      </c>
+    </row>
+    <row r="337" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E337" t="s">
+        <v>17</v>
+      </c>
+      <c r="G337">
+        <f>G335+I331</f>
+        <v>2.2016918172404171E-2</v>
+      </c>
+      <c r="K337">
+        <f>G337*J335</f>
+        <v>8.1462597237895437E-2</v>
+      </c>
+    </row>
+    <row r="338" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E338" t="s">
+        <v>18</v>
+      </c>
+      <c r="G338">
+        <f>H329+I332</f>
+        <v>1.6314740722656251E-3</v>
+      </c>
+      <c r="K338">
+        <f>G338*J335</f>
+        <v>6.036454067382813E-3</v>
       </c>
     </row>
   </sheetData>
@@ -25518,10 +25777,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L332"/>
+  <dimension ref="A1:O338"/>
   <sheetViews>
-    <sheetView topLeftCell="A310" workbookViewId="0">
-      <selection activeCell="D327" sqref="D327:L332"/>
+    <sheetView topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="H309" sqref="H309:L312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25535,21 +25794,21 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -37586,7 +37845,7 @@
         <v>298.4716796875</v>
       </c>
     </row>
-    <row r="306" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="306" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D306" t="s">
         <v>9</v>
       </c>
@@ -37595,7 +37854,7 @@
         <v>295.71673583984375</v>
       </c>
     </row>
-    <row r="308" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="308" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D308" t="s">
         <v>10</v>
       </c>
@@ -37615,83 +37874,83 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="309" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H309">
-        <f>20*10^-6</f>
-        <v>1.9999999999999998E-5</v>
+        <f>20*10^-3</f>
+        <v>0.02</v>
       </c>
       <c r="K309">
-        <f>24*10^-6</f>
-        <v>2.4000000000000001E-5</v>
+        <f>24*10^-3</f>
+        <v>2.4E-2</v>
       </c>
       <c r="L309">
-        <f>20*10^-6</f>
-        <v>1.9999999999999998E-5</v>
-      </c>
-    </row>
-    <row r="310" spans="4:12" x14ac:dyDescent="0.3">
+        <f>20*10^-3</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="310" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E310" t="s">
         <v>16</v>
       </c>
       <c r="I310">
-        <f>0.6*10^-6</f>
-        <v>5.9999999999999997E-7</v>
-      </c>
-    </row>
-    <row r="311" spans="4:12" x14ac:dyDescent="0.3">
+        <f>0.6*10^-3</f>
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="311" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E311" t="s">
         <v>17</v>
       </c>
       <c r="I311">
-        <f>1.3*10^-9</f>
-        <v>1.3000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="312" spans="4:12" x14ac:dyDescent="0.3">
+        <f>1.3*10^-6</f>
+        <v>1.3E-6</v>
+      </c>
+    </row>
+    <row r="312" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E312" t="s">
         <v>18</v>
       </c>
       <c r="I312">
-        <f>0.4*10^-9</f>
-        <v>4.0000000000000007E-10</v>
-      </c>
-    </row>
-    <row r="314" spans="4:12" x14ac:dyDescent="0.3">
+        <f>0.4*10^-6</f>
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="314" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D314" t="s">
         <v>19</v>
       </c>
       <c r="H314">
         <f>H303*H309</f>
-        <v>7.9890136718749992E-5</v>
+        <v>7.9890136718750004E-2</v>
       </c>
       <c r="K314">
         <f>K303*K309</f>
-        <v>1.2705322265625001E-5</v>
+        <v>1.2705322265625001E-2</v>
       </c>
       <c r="L314">
         <f>L303*L309</f>
-        <v>5.9694335937499994E-3</v>
-      </c>
-    </row>
-    <row r="315" spans="4:12" x14ac:dyDescent="0.3">
+        <v>5.9694335937499998</v>
+      </c>
+    </row>
+    <row r="315" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I315">
         <f>I306*I310</f>
-        <v>1.7743004150390623E-4</v>
-      </c>
-    </row>
-    <row r="316" spans="4:12" x14ac:dyDescent="0.3">
+        <v>0.17743004150390623</v>
+      </c>
+    </row>
+    <row r="316" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I316">
         <f>I306*I311</f>
-        <v>3.8443175659179691E-7</v>
-      </c>
-    </row>
-    <row r="317" spans="4:12" x14ac:dyDescent="0.3">
+        <v>3.8443175659179688E-4</v>
+      </c>
+    </row>
+    <row r="317" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I317">
         <f>I306*I312</f>
-        <v>1.1828669433593752E-7</v>
-      </c>
-    </row>
-    <row r="320" spans="4:12" x14ac:dyDescent="0.3">
+        <v>1.182866943359375E-4</v>
+      </c>
+    </row>
+    <row r="320" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D320" t="s">
         <v>20</v>
       </c>
@@ -37700,37 +37959,78 @@
       </c>
       <c r="G320">
         <f>H309+K309+L309</f>
-        <v>6.3999999999999997E-5</v>
-      </c>
-    </row>
-    <row r="321" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="I320" t="s">
+        <v>23</v>
+      </c>
+      <c r="J320">
+        <v>3.7</v>
+      </c>
+      <c r="K320">
+        <f>J320*G320</f>
+        <v>0.23680000000000001</v>
+      </c>
+      <c r="M320" t="s">
+        <v>24</v>
+      </c>
+      <c r="N320">
+        <f>(K320/12) * 1000</f>
+        <v>19.733333333333334</v>
+      </c>
+    </row>
+    <row r="321" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E321" t="s">
         <v>16</v>
       </c>
       <c r="G321">
         <f>G320+I310</f>
-        <v>6.4599999999999998E-5</v>
-      </c>
-    </row>
-    <row r="322" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4600000000000005E-2</v>
+      </c>
+      <c r="K321">
+        <f>G321*J320</f>
+        <v>0.23902000000000004</v>
+      </c>
+      <c r="N321">
+        <f>(K321/12) * 1000</f>
+        <v>19.918333333333337</v>
+      </c>
+    </row>
+    <row r="322" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E322" t="s">
         <v>17</v>
       </c>
       <c r="G322">
         <f>G320+I311</f>
-        <v>6.4001299999999993E-5</v>
-      </c>
-    </row>
-    <row r="323" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4001299999999997E-2</v>
+      </c>
+      <c r="K322">
+        <f>G322*J320</f>
+        <v>0.23680481</v>
+      </c>
+      <c r="N322">
+        <f>(K322/12) * 1000</f>
+        <v>19.733734166666665</v>
+      </c>
+    </row>
+    <row r="323" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E323" t="s">
         <v>18</v>
       </c>
       <c r="G323">
         <f>G320+I312</f>
-        <v>6.4000399999999998E-5</v>
-      </c>
-    </row>
-    <row r="327" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4000399999999999E-2</v>
+      </c>
+      <c r="K323">
+        <f>G323*J320</f>
+        <v>0.23680148000000001</v>
+      </c>
+      <c r="N323">
+        <f>(K323/12) * 1000</f>
+        <v>19.733456666666665</v>
+      </c>
+    </row>
+    <row r="327" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D327" t="s">
         <v>22</v>
       </c>
@@ -37751,48 +38051,127 @@
         <v>0.998199462890625</v>
       </c>
     </row>
-    <row r="329" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="329" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D329" t="s">
         <v>19</v>
       </c>
       <c r="H329">
         <f>H309*H314</f>
-        <v>1.5978027343749998E-9</v>
+        <v>1.5978027343750002E-3</v>
       </c>
       <c r="K329">
         <f>K327*K309</f>
-        <v>4.248046875E-8</v>
+        <v>4.2480468750000004E-5</v>
       </c>
       <c r="L329">
         <f>L309*L327</f>
-        <v>1.99639892578125E-5</v>
-      </c>
-    </row>
-    <row r="330" spans="4:12" x14ac:dyDescent="0.3">
+        <v>1.9963989257812502E-2</v>
+      </c>
+      <c r="N329" t="s">
+        <v>23</v>
+      </c>
+      <c r="O329">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="330" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E330" t="s">
         <v>16</v>
       </c>
       <c r="I330">
         <f>I310*I327</f>
-        <v>5.9470825195312495E-7</v>
-      </c>
-    </row>
-    <row r="331" spans="4:12" x14ac:dyDescent="0.3">
+        <v>5.9470825195312492E-4</v>
+      </c>
+      <c r="O330" s="1">
+        <f>I330*O329</f>
+        <v>2.2004205322265621E-3</v>
+      </c>
+    </row>
+    <row r="331" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E331" t="s">
         <v>17</v>
       </c>
       <c r="I331">
         <f>I316*I327</f>
-        <v>3.8104122992996127E-7</v>
-      </c>
-    </row>
-    <row r="332" spans="4:12" x14ac:dyDescent="0.3">
+        <v>3.8104122992996129E-4</v>
+      </c>
+      <c r="O331" s="1">
+        <f>I331*O329</f>
+        <v>1.4098525507408568E-3</v>
+      </c>
+    </row>
+    <row r="332" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E332" t="s">
         <v>18</v>
       </c>
       <c r="I332">
         <f>I312*I327</f>
-        <v>3.9647216796875009E-10</v>
+        <v>3.9647216796874997E-7</v>
+      </c>
+      <c r="O332" s="1">
+        <f>I332*O329</f>
+        <v>1.466947021484375E-6</v>
+      </c>
+    </row>
+    <row r="335" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D335" t="s">
+        <v>20</v>
+      </c>
+      <c r="E335" t="s">
+        <v>21</v>
+      </c>
+      <c r="G335">
+        <f>H329+K329+L329</f>
+        <v>2.1604272460937501E-2</v>
+      </c>
+      <c r="I335" t="s">
+        <v>23</v>
+      </c>
+      <c r="J335">
+        <v>3.7</v>
+      </c>
+      <c r="K335">
+        <f>G335*J335</f>
+        <v>7.9935808105468756E-2</v>
+      </c>
+    </row>
+    <row r="336" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="E336" t="s">
+        <v>16</v>
+      </c>
+      <c r="G336">
+        <f>G335+I330</f>
+        <v>2.2198980712890625E-2</v>
+      </c>
+      <c r="K336">
+        <f>G336*J335</f>
+        <v>8.2136228637695319E-2</v>
+      </c>
+    </row>
+    <row r="337" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E337" t="s">
+        <v>17</v>
+      </c>
+      <c r="G337">
+        <f>G335+I331</f>
+        <v>2.1985313690867463E-2</v>
+      </c>
+      <c r="K337">
+        <f>G337*J335</f>
+        <v>8.1345660656209615E-2</v>
+      </c>
+    </row>
+    <row r="338" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E338" t="s">
+        <v>18</v>
+      </c>
+      <c r="G338">
+        <f>H329+I332</f>
+        <v>1.5981992065429689E-3</v>
+      </c>
+      <c r="K338">
+        <f>G338*J335</f>
+        <v>5.9133370642089856E-3</v>
       </c>
     </row>
   </sheetData>
@@ -37806,10 +38185,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L332"/>
+  <dimension ref="A1:O338"/>
   <sheetViews>
-    <sheetView topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="D327" sqref="D327:L332"/>
+    <sheetView topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="H309" sqref="H309:L312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37823,21 +38202,21 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -49874,7 +50253,7 @@
         <v>298.47171020507813</v>
       </c>
     </row>
-    <row r="306" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="306" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D306" t="s">
         <v>9</v>
       </c>
@@ -49883,7 +50262,7 @@
         <v>295.72354125976563</v>
       </c>
     </row>
-    <row r="308" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="308" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D308" t="s">
         <v>10</v>
       </c>
@@ -49903,83 +50282,83 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="309" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H309">
-        <f>20*10^-6</f>
-        <v>1.9999999999999998E-5</v>
+        <f>20*10^-3</f>
+        <v>0.02</v>
       </c>
       <c r="K309">
-        <f>24*10^-6</f>
-        <v>2.4000000000000001E-5</v>
+        <f>24*10^-3</f>
+        <v>2.4E-2</v>
       </c>
       <c r="L309">
-        <f>20*10^-6</f>
-        <v>1.9999999999999998E-5</v>
-      </c>
-    </row>
-    <row r="310" spans="4:12" x14ac:dyDescent="0.3">
+        <f>20*10^-3</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="310" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E310" t="s">
         <v>16</v>
       </c>
       <c r="I310">
-        <f>0.6*10^-6</f>
-        <v>5.9999999999999997E-7</v>
-      </c>
-    </row>
-    <row r="311" spans="4:12" x14ac:dyDescent="0.3">
+        <f>0.6*10^-3</f>
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="311" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E311" t="s">
         <v>17</v>
       </c>
       <c r="I311">
-        <f>1.3*10^-9</f>
-        <v>1.3000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="312" spans="4:12" x14ac:dyDescent="0.3">
+        <f>1.3*10^-6</f>
+        <v>1.3E-6</v>
+      </c>
+    </row>
+    <row r="312" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E312" t="s">
         <v>18</v>
       </c>
       <c r="I312">
-        <f>0.4*10^-9</f>
-        <v>4.0000000000000007E-10</v>
-      </c>
-    </row>
-    <row r="314" spans="4:12" x14ac:dyDescent="0.3">
+        <f>0.4*10^-6</f>
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="314" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D314" t="s">
         <v>19</v>
       </c>
       <c r="H314">
         <f>H303*H309</f>
-        <v>7.9741821289062496E-5</v>
+        <v>7.9741821289062501E-2</v>
       </c>
       <c r="K314">
         <f>K303*K309</f>
-        <v>1.270458984375E-5</v>
+        <v>1.2704589843750001E-2</v>
       </c>
       <c r="L314">
         <f>L303*L309</f>
-        <v>5.9694342041015621E-3</v>
-      </c>
-    </row>
-    <row r="315" spans="4:12" x14ac:dyDescent="0.3">
+        <v>5.9694342041015629</v>
+      </c>
+    </row>
+    <row r="315" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I315">
         <f>I306*I310</f>
-        <v>1.7743412475585937E-4</v>
-      </c>
-    </row>
-    <row r="316" spans="4:12" x14ac:dyDescent="0.3">
+        <v>0.17743412475585935</v>
+      </c>
+    </row>
+    <row r="316" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I316">
         <f>I306*I311</f>
-        <v>3.8444060363769536E-7</v>
-      </c>
-    </row>
-    <row r="317" spans="4:12" x14ac:dyDescent="0.3">
+        <v>3.8444060363769533E-4</v>
+      </c>
+    </row>
+    <row r="317" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I317">
         <f>I306*I312</f>
-        <v>1.1828941650390627E-7</v>
-      </c>
-    </row>
-    <row r="320" spans="4:12" x14ac:dyDescent="0.3">
+        <v>1.1828941650390624E-4</v>
+      </c>
+    </row>
+    <row r="320" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D320" t="s">
         <v>20</v>
       </c>
@@ -49988,37 +50367,78 @@
       </c>
       <c r="G320">
         <f>H309+K309+L309</f>
-        <v>6.3999999999999997E-5</v>
-      </c>
-    </row>
-    <row r="321" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="I320" t="s">
+        <v>23</v>
+      </c>
+      <c r="J320">
+        <v>3.7</v>
+      </c>
+      <c r="K320">
+        <f>J320*G320</f>
+        <v>0.23680000000000001</v>
+      </c>
+      <c r="M320" t="s">
+        <v>24</v>
+      </c>
+      <c r="N320">
+        <f>(K320/12) * 1000</f>
+        <v>19.733333333333334</v>
+      </c>
+    </row>
+    <row r="321" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E321" t="s">
         <v>16</v>
       </c>
       <c r="G321">
         <f>G320+I310</f>
-        <v>6.4599999999999998E-5</v>
-      </c>
-    </row>
-    <row r="322" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4600000000000005E-2</v>
+      </c>
+      <c r="K321">
+        <f>G321*J320</f>
+        <v>0.23902000000000004</v>
+      </c>
+      <c r="N321">
+        <f>(K321/12) * 1000</f>
+        <v>19.918333333333337</v>
+      </c>
+    </row>
+    <row r="322" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E322" t="s">
         <v>17</v>
       </c>
       <c r="G322">
         <f>G320+I311</f>
-        <v>6.4001299999999993E-5</v>
-      </c>
-    </row>
-    <row r="323" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4001299999999997E-2</v>
+      </c>
+      <c r="K322">
+        <f>G322*J320</f>
+        <v>0.23680481</v>
+      </c>
+      <c r="N322">
+        <f>(K322/12) * 1000</f>
+        <v>19.733734166666665</v>
+      </c>
+    </row>
+    <row r="323" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E323" t="s">
         <v>18</v>
       </c>
       <c r="G323">
         <f>G320+I312</f>
-        <v>6.4000399999999998E-5</v>
-      </c>
-    </row>
-    <row r="327" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4000399999999999E-2</v>
+      </c>
+      <c r="K323">
+        <f>G323*J320</f>
+        <v>0.23680148000000001</v>
+      </c>
+      <c r="N323">
+        <f>(K323/12) * 1000</f>
+        <v>19.733456666666665</v>
+      </c>
+    </row>
+    <row r="327" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D327" t="s">
         <v>22</v>
       </c>
@@ -50039,48 +50459,127 @@
         <v>0.99822998046875</v>
       </c>
     </row>
-    <row r="329" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="329" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D329" t="s">
         <v>19</v>
       </c>
       <c r="H329">
         <f>H309*H314</f>
-        <v>1.5948364257812497E-9</v>
+        <v>1.59483642578125E-3</v>
       </c>
       <c r="K329">
         <f>K327*K309</f>
-        <v>4.248046875E-8</v>
+        <v>4.2480468750000004E-5</v>
       </c>
       <c r="L329">
         <f>L309*L327</f>
-        <v>1.9964599609374997E-5</v>
-      </c>
-    </row>
-    <row r="330" spans="4:12" x14ac:dyDescent="0.3">
+        <v>1.9964599609375001E-2</v>
+      </c>
+      <c r="N329" t="s">
+        <v>23</v>
+      </c>
+      <c r="O329">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="330" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E330" t="s">
         <v>16</v>
       </c>
       <c r="I330">
         <f>I310*I327</f>
-        <v>5.92401123046875E-7</v>
-      </c>
-    </row>
-    <row r="331" spans="4:12" x14ac:dyDescent="0.3">
+        <v>5.9240112304687498E-4</v>
+      </c>
+      <c r="O330" s="1">
+        <f>I330*O329</f>
+        <v>2.1918841552734376E-3</v>
+      </c>
+    </row>
+    <row r="331" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E331" t="s">
         <v>17</v>
       </c>
       <c r="I331">
         <f>I316*I327</f>
-        <v>3.795717422329821E-7</v>
-      </c>
-    </row>
-    <row r="332" spans="4:12" x14ac:dyDescent="0.3">
+        <v>3.795717422329821E-4</v>
+      </c>
+      <c r="O331" s="1">
+        <f>I331*O329</f>
+        <v>1.4044154462620338E-3</v>
+      </c>
+    </row>
+    <row r="332" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E332" t="s">
         <v>18</v>
       </c>
       <c r="I332">
         <f>I312*I327</f>
-        <v>3.9493408203125007E-10</v>
+        <v>3.9493408203125E-7</v>
+      </c>
+      <c r="O332" s="1">
+        <f>I332*O329</f>
+        <v>1.4612561035156252E-6</v>
+      </c>
+    </row>
+    <row r="335" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D335" t="s">
+        <v>20</v>
+      </c>
+      <c r="E335" t="s">
+        <v>21</v>
+      </c>
+      <c r="G335">
+        <f>H329+K329+L329</f>
+        <v>2.1601916503906252E-2</v>
+      </c>
+      <c r="I335" t="s">
+        <v>23</v>
+      </c>
+      <c r="J335">
+        <v>3.7</v>
+      </c>
+      <c r="K335">
+        <f>G335*J335</f>
+        <v>7.9927091064453143E-2</v>
+      </c>
+    </row>
+    <row r="336" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="E336" t="s">
+        <v>16</v>
+      </c>
+      <c r="G336">
+        <f>G335+I330</f>
+        <v>2.2194317626953126E-2</v>
+      </c>
+      <c r="K336">
+        <f>G336*J335</f>
+        <v>8.2118975219726567E-2</v>
+      </c>
+    </row>
+    <row r="337" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E337" t="s">
+        <v>17</v>
+      </c>
+      <c r="G337">
+        <f>G335+I331</f>
+        <v>2.1981488246139234E-2</v>
+      </c>
+      <c r="K337">
+        <f>G337*J335</f>
+        <v>8.1331506510715176E-2</v>
+      </c>
+    </row>
+    <row r="338" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E338" t="s">
+        <v>18</v>
+      </c>
+      <c r="G338">
+        <f>H329+I332</f>
+        <v>1.5952313598632812E-3</v>
+      </c>
+      <c r="K338">
+        <f>G338*J335</f>
+        <v>5.9023560314941407E-3</v>
       </c>
     </row>
   </sheetData>
@@ -50094,16 +50593,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:L332"/>
+  <dimension ref="A1:O338"/>
   <sheetViews>
-    <sheetView topLeftCell="A306" workbookViewId="0">
-      <selection activeCell="D327" sqref="D327:L332"/>
+    <sheetView tabSelected="1" topLeftCell="E298" workbookViewId="0">
+      <selection activeCell="L309" sqref="L309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -50115,21 +50615,21 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -62166,7 +62666,7 @@
         <v>298.4716796875</v>
       </c>
     </row>
-    <row r="306" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="306" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D306" t="s">
         <v>9</v>
       </c>
@@ -62175,7 +62675,7 @@
         <v>295.72064208984375</v>
       </c>
     </row>
-    <row r="308" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="308" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D308" t="s">
         <v>10</v>
       </c>
@@ -62195,83 +62695,86 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="309" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H309">
-        <f>20*10^-6</f>
-        <v>1.9999999999999998E-5</v>
+        <f>20*10^-3</f>
+        <v>0.02</v>
       </c>
       <c r="K309">
-        <f>24*10^-6</f>
-        <v>2.4000000000000001E-5</v>
+        <f>24*10^-3</f>
+        <v>2.4E-2</v>
       </c>
       <c r="L309">
-        <f>20*10^-6</f>
-        <v>1.9999999999999998E-5</v>
-      </c>
-    </row>
-    <row r="310" spans="4:12" x14ac:dyDescent="0.3">
+        <f>20*10^-3</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="310" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E310" t="s">
         <v>16</v>
       </c>
       <c r="I310">
-        <f>0.6*10^-6</f>
-        <v>5.9999999999999997E-7</v>
-      </c>
-    </row>
-    <row r="311" spans="4:12" x14ac:dyDescent="0.3">
+        <f>0.6*10^-3</f>
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="311" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E311" t="s">
         <v>17</v>
       </c>
       <c r="I311">
-        <f>1.3*10^-9</f>
-        <v>1.3000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="312" spans="4:12" x14ac:dyDescent="0.3">
+        <f>1.3*10^-6</f>
+        <v>1.3E-6</v>
+      </c>
+    </row>
+    <row r="312" spans="4:14" x14ac:dyDescent="0.3">
       <c r="E312" t="s">
         <v>18</v>
       </c>
       <c r="I312">
-        <f>0.4*10^-9</f>
-        <v>4.0000000000000007E-10</v>
-      </c>
-    </row>
-    <row r="314" spans="4:12" x14ac:dyDescent="0.3">
+        <f>0.4*10^-6</f>
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="314" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D314" t="s">
         <v>19</v>
       </c>
+      <c r="G314" t="s">
+        <v>25</v>
+      </c>
       <c r="H314">
         <f>H303*H309</f>
-        <v>7.9812011718749995E-5</v>
+        <v>7.9812011718750006E-2</v>
       </c>
       <c r="K314">
         <f>K303*K309</f>
-        <v>1.2705322265625001E-5</v>
+        <v>1.2705322265625001E-2</v>
       </c>
       <c r="L314">
         <f>L303*L309</f>
-        <v>5.9694335937499994E-3</v>
-      </c>
-    </row>
-    <row r="315" spans="4:12" x14ac:dyDescent="0.3">
+        <v>5.9694335937499998</v>
+      </c>
+    </row>
+    <row r="315" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I315">
         <f>I306*I310</f>
-        <v>1.7743238525390624E-4</v>
-      </c>
-    </row>
-    <row r="316" spans="4:12" x14ac:dyDescent="0.3">
+        <v>0.17743238525390623</v>
+      </c>
+    </row>
+    <row r="316" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I316">
         <f>I306*I311</f>
-        <v>3.8443683471679689E-7</v>
-      </c>
-    </row>
-    <row r="317" spans="4:12" x14ac:dyDescent="0.3">
+        <v>3.8443683471679687E-4</v>
+      </c>
+    </row>
+    <row r="317" spans="4:14" x14ac:dyDescent="0.3">
       <c r="I317">
         <f>I306*I312</f>
-        <v>1.1828825683593753E-7</v>
-      </c>
-    </row>
-    <row r="320" spans="4:12" x14ac:dyDescent="0.3">
+        <v>1.1828825683593749E-4</v>
+      </c>
+    </row>
+    <row r="320" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D320" t="s">
         <v>20</v>
       </c>
@@ -62280,37 +62783,78 @@
       </c>
       <c r="G320">
         <f>H309+K309+L309</f>
-        <v>6.3999999999999997E-5</v>
-      </c>
-    </row>
-    <row r="321" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="I320" t="s">
+        <v>23</v>
+      </c>
+      <c r="J320">
+        <v>3.7</v>
+      </c>
+      <c r="K320">
+        <f>J320*G320</f>
+        <v>0.23680000000000001</v>
+      </c>
+      <c r="M320" t="s">
+        <v>24</v>
+      </c>
+      <c r="N320">
+        <f>(K320/12) * 1000</f>
+        <v>19.733333333333334</v>
+      </c>
+    </row>
+    <row r="321" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E321" t="s">
         <v>16</v>
       </c>
       <c r="G321">
         <f>G320+I310</f>
-        <v>6.4599999999999998E-5</v>
-      </c>
-    </row>
-    <row r="322" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4600000000000005E-2</v>
+      </c>
+      <c r="K321">
+        <f>G321*J320</f>
+        <v>0.23902000000000004</v>
+      </c>
+      <c r="N321">
+        <f>(K321/12) * 1000</f>
+        <v>19.918333333333337</v>
+      </c>
+    </row>
+    <row r="322" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E322" t="s">
         <v>17</v>
       </c>
       <c r="G322">
         <f>G320+I311</f>
-        <v>6.4001299999999993E-5</v>
-      </c>
-    </row>
-    <row r="323" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4001299999999997E-2</v>
+      </c>
+      <c r="K322">
+        <f>G322*J320</f>
+        <v>0.23680481</v>
+      </c>
+      <c r="N322">
+        <f>(K322/12) * 1000</f>
+        <v>19.733734166666665</v>
+      </c>
+    </row>
+    <row r="323" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E323" t="s">
         <v>18</v>
       </c>
       <c r="G323">
         <f>G320+I312</f>
-        <v>6.4000399999999998E-5</v>
-      </c>
-    </row>
-    <row r="327" spans="4:12" x14ac:dyDescent="0.3">
+        <v>6.4000399999999999E-2</v>
+      </c>
+      <c r="K323">
+        <f>G323*J320</f>
+        <v>0.23680148000000001</v>
+      </c>
+      <c r="N323">
+        <f>(K323/12) * 1000</f>
+        <v>19.733456666666665</v>
+      </c>
+    </row>
+    <row r="327" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D327" t="s">
         <v>22</v>
       </c>
@@ -62331,48 +62875,127 @@
         <v>0.99822998046875</v>
       </c>
     </row>
-    <row r="329" spans="4:12" x14ac:dyDescent="0.3">
+    <row r="329" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D329" t="s">
         <v>19</v>
       </c>
       <c r="H329">
         <f>H309*H314</f>
-        <v>1.5962402343749997E-9</v>
+        <v>1.5962402343750002E-3</v>
       </c>
       <c r="K329">
         <f>K327*K309</f>
-        <v>4.248046875E-8</v>
+        <v>4.2480468750000004E-5</v>
       </c>
       <c r="L329">
         <f>L309*L327</f>
-        <v>1.9964599609374997E-5</v>
-      </c>
-    </row>
-    <row r="330" spans="4:12" x14ac:dyDescent="0.3">
+        <v>1.9964599609375001E-2</v>
+      </c>
+      <c r="N329" t="s">
+        <v>23</v>
+      </c>
+      <c r="O329">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="330" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E330" t="s">
         <v>16</v>
       </c>
       <c r="I330">
         <f>I310*I327</f>
-        <v>5.92401123046875E-7</v>
-      </c>
-    </row>
-    <row r="331" spans="4:12" x14ac:dyDescent="0.3">
+        <v>5.9240112304687498E-4</v>
+      </c>
+      <c r="O330" s="1">
+        <f>I330*O329</f>
+        <v>2.1918841552734376E-3</v>
+      </c>
+    </row>
+    <row r="331" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E331" t="s">
         <v>17</v>
       </c>
       <c r="I331">
         <f>I316*I327</f>
-        <v>3.7956802104469388E-7</v>
-      </c>
-    </row>
-    <row r="332" spans="4:12" x14ac:dyDescent="0.3">
+        <v>3.7956802104469387E-4</v>
+      </c>
+      <c r="O331" s="1">
+        <f>I331*O329</f>
+        <v>1.4044016778653674E-3</v>
+      </c>
+    </row>
+    <row r="332" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E332" t="s">
         <v>18</v>
       </c>
       <c r="I332">
         <f>I312*I327</f>
-        <v>3.9493408203125007E-10</v>
+        <v>3.9493408203125E-7</v>
+      </c>
+      <c r="O332" s="1">
+        <f>I332*O329</f>
+        <v>1.4612561035156252E-6</v>
+      </c>
+    </row>
+    <row r="335" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D335" t="s">
+        <v>20</v>
+      </c>
+      <c r="E335" t="s">
+        <v>21</v>
+      </c>
+      <c r="G335">
+        <f>H329+K329+L329</f>
+        <v>2.16033203125E-2</v>
+      </c>
+      <c r="I335" t="s">
+        <v>23</v>
+      </c>
+      <c r="J335">
+        <v>3.7</v>
+      </c>
+      <c r="K335">
+        <f>G335*J335</f>
+        <v>7.9932285156250005E-2</v>
+      </c>
+    </row>
+    <row r="336" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="E336" t="s">
+        <v>16</v>
+      </c>
+      <c r="G336">
+        <f>G335+I330</f>
+        <v>2.2195721435546874E-2</v>
+      </c>
+      <c r="K336">
+        <f>G336*J335</f>
+        <v>8.2124169311523443E-2</v>
+      </c>
+    </row>
+    <row r="337" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E337" t="s">
+        <v>17</v>
+      </c>
+      <c r="G337">
+        <f>G335+I331</f>
+        <v>2.1982888333544694E-2</v>
+      </c>
+      <c r="K337">
+        <f>G337*J335</f>
+        <v>8.1336686834115379E-2</v>
+      </c>
+    </row>
+    <row r="338" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E338" t="s">
+        <v>18</v>
+      </c>
+      <c r="G338">
+        <f>H329+I332</f>
+        <v>1.5966351684570314E-3</v>
+      </c>
+      <c r="K338">
+        <f>G338*J335</f>
+        <v>5.9075501232910164E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed the energest conversion
</commit_message>
<xml_diff>
--- a/datalogging/power consumption/energest/converted2_4-merged.xlsx
+++ b/datalogging/power consumption/energest/converted2_4-merged.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Univ\SensorManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67645C8-B5CC-42ED-B38A-A1A69A701A3C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47129A45-4229-4296-B5EF-70C74D72A491}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="29">
   <si>
     <t>packet</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>joule to mWh:</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Energy</t>
   </si>
 </sst>
 </file>
@@ -952,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O338"/>
+  <dimension ref="A1:S338"/>
   <sheetViews>
-    <sheetView topLeftCell="A295" workbookViewId="0">
-      <selection activeCell="H309" sqref="H309:L312"/>
+    <sheetView topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="K319" sqref="K319:N319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13025,7 +13034,7 @@
         <v>298.46636962890625</v>
       </c>
     </row>
-    <row r="306" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="306" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D306" t="s">
         <v>9</v>
       </c>
@@ -13034,7 +13043,7 @@
         <v>295.73062133789063</v>
       </c>
     </row>
-    <row r="308" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="308" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D308" t="s">
         <v>10</v>
       </c>
@@ -13054,7 +13063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="309" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H309">
         <f>20*10^-3</f>
         <v>0.02</v>
@@ -13068,7 +13077,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="310" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="310" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E310" t="s">
         <v>16</v>
       </c>
@@ -13077,7 +13086,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="311" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="311" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E311" t="s">
         <v>17</v>
       </c>
@@ -13086,7 +13095,7 @@
         <v>1.3E-6</v>
       </c>
     </row>
-    <row r="312" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="312" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E312" t="s">
         <v>18</v>
       </c>
@@ -13095,7 +13104,7 @@
         <v>3.9999999999999998E-7</v>
       </c>
     </row>
-    <row r="314" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="314" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D314" t="s">
         <v>19</v>
       </c>
@@ -13112,25 +13121,33 @@
         <v>5.9693273925781254</v>
       </c>
     </row>
-    <row r="315" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="315" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I315">
         <f>I306*I310</f>
         <v>0.17743837280273436</v>
       </c>
     </row>
-    <row r="316" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="316" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I316">
         <f>I306*I311</f>
         <v>3.8444980773925784E-4</v>
       </c>
     </row>
-    <row r="317" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="317" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I317">
         <f>I306*I312</f>
         <v>1.1829224853515624E-4</v>
       </c>
     </row>
-    <row r="320" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="319" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="K319" t="s">
+        <v>27</v>
+      </c>
+      <c r="N319" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="320" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D320" t="s">
         <v>20</v>
       </c>
@@ -13138,8 +13155,8 @@
         <v>21</v>
       </c>
       <c r="G320">
-        <f>H309+K309+L309</f>
-        <v>6.4000000000000001E-2</v>
+        <f>H314+K314+L314</f>
+        <v>6.0617603759765633</v>
       </c>
       <c r="I320" t="s">
         <v>23</v>
@@ -13149,18 +13166,21 @@
       </c>
       <c r="K320">
         <f>J320*G320</f>
-        <v>0.23680000000000001</v>
+        <v>22.428513391113285</v>
       </c>
       <c r="M320" t="s">
         <v>24</v>
       </c>
       <c r="N320">
-        <f>(K320/12) * 1000</f>
-        <v>19.733333333333334</v>
-      </c>
-      <c r="O320">
-        <f>(K320*1000)/12</f>
-        <v>19.733333333333334</v>
+        <f>K320*S320</f>
+        <v>6.2301408642026486</v>
+      </c>
+      <c r="Q320" t="s">
+        <v>26</v>
+      </c>
+      <c r="S320">
+        <f>0.2777777</f>
+        <v>0.27777770000000002</v>
       </c>
     </row>
     <row r="321" spans="4:15" x14ac:dyDescent="0.3">
@@ -13168,16 +13188,16 @@
         <v>16</v>
       </c>
       <c r="G321">
-        <f>G320+I310</f>
-        <v>6.4600000000000005E-2</v>
+        <f>G320+I315</f>
+        <v>6.2391987487792973</v>
       </c>
       <c r="K321">
         <f>G321*J320</f>
-        <v>0.23902000000000004</v>
+        <v>23.0850353704834</v>
       </c>
       <c r="N321">
-        <f>(K321/12) * 1000</f>
-        <v>19.918333333333337</v>
+        <f>K321*S320</f>
+        <v>6.4125080296315273</v>
       </c>
     </row>
     <row r="322" spans="4:15" x14ac:dyDescent="0.3">
@@ -13185,16 +13205,16 @@
         <v>17</v>
       </c>
       <c r="G322">
-        <f>G320+I311</f>
-        <v>6.4001299999999997E-2</v>
+        <f>G320+I316</f>
+        <v>6.0621448257843022</v>
       </c>
       <c r="K322">
         <f>G322*J320</f>
-        <v>0.23680481</v>
+        <v>22.429935855401919</v>
       </c>
       <c r="N322">
-        <f>(K322/12) * 1000</f>
-        <v>19.733734166666665</v>
+        <f>K322*S320</f>
+        <v>6.2305359930610775</v>
       </c>
     </row>
     <row r="323" spans="4:15" x14ac:dyDescent="0.3">
@@ -13202,16 +13222,16 @@
         <v>18</v>
       </c>
       <c r="G323">
-        <f>G320+I312</f>
-        <v>6.4000399999999999E-2</v>
+        <f>G320+I317</f>
+        <v>6.0618786682250985</v>
       </c>
       <c r="K323">
         <f>G323*J320</f>
-        <v>0.23680148000000001</v>
+        <v>22.428951072432866</v>
       </c>
       <c r="N323">
-        <f>(K323/12) * 1000</f>
-        <v>19.733456666666665</v>
+        <f>K323*S320</f>
+        <v>6.2302624423129354</v>
       </c>
     </row>
     <row r="327" spans="4:15" x14ac:dyDescent="0.3">
@@ -13369,10 +13389,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O338"/>
+  <dimension ref="A1:S338"/>
   <sheetViews>
     <sheetView topLeftCell="A299" workbookViewId="0">
-      <selection activeCell="H309" sqref="H309:L312"/>
+      <selection activeCell="K319" sqref="K319:N319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25437,7 +25457,7 @@
         <v>298.4718017578125</v>
       </c>
     </row>
-    <row r="306" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="306" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D306" t="s">
         <v>9</v>
       </c>
@@ -25446,7 +25466,7 @@
         <v>295.633544921875</v>
       </c>
     </row>
-    <row r="308" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="308" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D308" t="s">
         <v>10</v>
       </c>
@@ -25466,7 +25486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="309" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H309">
         <f>20*10^-3</f>
         <v>0.02</v>
@@ -25480,7 +25500,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="310" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="310" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E310" t="s">
         <v>16</v>
       </c>
@@ -25489,7 +25509,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="311" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="311" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E311" t="s">
         <v>17</v>
       </c>
@@ -25498,7 +25518,7 @@
         <v>1.3E-6</v>
       </c>
     </row>
-    <row r="312" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="312" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E312" t="s">
         <v>18</v>
       </c>
@@ -25507,7 +25527,7 @@
         <v>3.9999999999999998E-7</v>
       </c>
     </row>
-    <row r="314" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="314" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D314" t="s">
         <v>19</v>
       </c>
@@ -25524,25 +25544,33 @@
         <v>5.9694360351562503</v>
       </c>
     </row>
-    <row r="315" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="315" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I315">
         <f>I306*I310</f>
         <v>0.17738012695312499</v>
       </c>
     </row>
-    <row r="316" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="316" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I316">
         <f>I306*I311</f>
         <v>3.8432360839843753E-4</v>
       </c>
     </row>
-    <row r="317" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="317" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I317">
         <f>I306*I312</f>
         <v>1.1825341796874999E-4</v>
       </c>
     </row>
-    <row r="320" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="319" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="K319" t="s">
+        <v>27</v>
+      </c>
+      <c r="N319" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="320" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D320" t="s">
         <v>20</v>
       </c>
@@ -25550,8 +25578,8 @@
         <v>21</v>
       </c>
       <c r="G320">
-        <f>H309+K309+L309</f>
-        <v>6.4000000000000001E-2</v>
+        <f>H314+K314+L314</f>
+        <v>6.0637106933593756</v>
       </c>
       <c r="I320" t="s">
         <v>23</v>
@@ -25561,14 +25589,21 @@
       </c>
       <c r="K320">
         <f>J320*G320</f>
-        <v>0.23680000000000001</v>
+        <v>22.435729565429693</v>
       </c>
       <c r="M320" t="s">
         <v>24</v>
       </c>
       <c r="N320">
-        <f>(K320/12) * 1000</f>
-        <v>19.733333333333334</v>
+        <f>K320*S320</f>
+        <v>6.2321453565070595</v>
+      </c>
+      <c r="Q320" t="s">
+        <v>26</v>
+      </c>
+      <c r="S320">
+        <f>0.2777777</f>
+        <v>0.27777770000000002</v>
       </c>
     </row>
     <row r="321" spans="4:15" x14ac:dyDescent="0.3">
@@ -25576,16 +25611,16 @@
         <v>16</v>
       </c>
       <c r="G321">
-        <f>G320+I310</f>
-        <v>6.4600000000000005E-2</v>
+        <f>G320+I315</f>
+        <v>6.2410908203125004</v>
       </c>
       <c r="K321">
         <f>G321*J320</f>
-        <v>0.23902000000000004</v>
+        <v>23.092036035156251</v>
       </c>
       <c r="N321">
-        <f>(K321/12) * 1000</f>
-        <v>19.918333333333337</v>
+        <f>K321*S320</f>
+        <v>6.4144526581628227</v>
       </c>
     </row>
     <row r="322" spans="4:15" x14ac:dyDescent="0.3">
@@ -25593,16 +25628,16 @@
         <v>17</v>
       </c>
       <c r="G322">
-        <f>G320+I311</f>
-        <v>6.4001299999999997E-2</v>
+        <f>G320+I316</f>
+        <v>6.0640950169677739</v>
       </c>
       <c r="K322">
         <f>G322*J320</f>
-        <v>0.23680481</v>
+        <v>22.437151562780766</v>
       </c>
       <c r="N322">
-        <f>(K322/12) * 1000</f>
-        <v>19.733734166666665</v>
+        <f>K322*S320</f>
+        <v>6.2325403556606469</v>
       </c>
     </row>
     <row r="323" spans="4:15" x14ac:dyDescent="0.3">
@@ -25610,16 +25645,16 @@
         <v>18</v>
       </c>
       <c r="G323">
-        <f>G320+I312</f>
-        <v>6.4000399999999999E-2</v>
+        <f>G320+I317</f>
+        <v>6.0638289467773445</v>
       </c>
       <c r="K323">
         <f>G323*J320</f>
-        <v>0.23680148000000001</v>
+        <v>22.436167103076176</v>
       </c>
       <c r="N323">
-        <f>(K323/12) * 1000</f>
-        <v>19.733456666666665</v>
+        <f>K323*S320</f>
+        <v>6.2322668947081636</v>
       </c>
     </row>
     <row r="327" spans="4:15" x14ac:dyDescent="0.3">
@@ -25777,10 +25812,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O338"/>
+  <dimension ref="A1:S338"/>
   <sheetViews>
     <sheetView topLeftCell="A304" workbookViewId="0">
-      <selection activeCell="H309" sqref="H309:L312"/>
+      <selection activeCell="K319" sqref="K319:N319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37845,7 +37880,7 @@
         <v>298.4716796875</v>
       </c>
     </row>
-    <row r="306" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="306" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D306" t="s">
         <v>9</v>
       </c>
@@ -37854,7 +37889,7 @@
         <v>295.71673583984375</v>
       </c>
     </row>
-    <row r="308" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="308" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D308" t="s">
         <v>10</v>
       </c>
@@ -37874,7 +37909,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="309" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H309">
         <f>20*10^-3</f>
         <v>0.02</v>
@@ -37888,7 +37923,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="310" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="310" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E310" t="s">
         <v>16</v>
       </c>
@@ -37897,7 +37932,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="311" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="311" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E311" t="s">
         <v>17</v>
       </c>
@@ -37906,7 +37941,7 @@
         <v>1.3E-6</v>
       </c>
     </row>
-    <row r="312" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="312" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E312" t="s">
         <v>18</v>
       </c>
@@ -37915,7 +37950,7 @@
         <v>3.9999999999999998E-7</v>
       </c>
     </row>
-    <row r="314" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="314" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D314" t="s">
         <v>19</v>
       </c>
@@ -37932,25 +37967,33 @@
         <v>5.9694335937499998</v>
       </c>
     </row>
-    <row r="315" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="315" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I315">
         <f>I306*I310</f>
         <v>0.17743004150390623</v>
       </c>
     </row>
-    <row r="316" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="316" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I316">
         <f>I306*I311</f>
         <v>3.8443175659179688E-4</v>
       </c>
     </row>
-    <row r="317" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="317" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I317">
         <f>I306*I312</f>
         <v>1.182866943359375E-4</v>
       </c>
     </row>
-    <row r="320" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="319" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="K319" t="s">
+        <v>27</v>
+      </c>
+      <c r="N319" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="320" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D320" t="s">
         <v>20</v>
       </c>
@@ -37958,8 +38001,8 @@
         <v>21</v>
       </c>
       <c r="G320">
-        <f>H309+K309+L309</f>
-        <v>6.4000000000000001E-2</v>
+        <f>H314+K314+L314</f>
+        <v>6.062029052734375</v>
       </c>
       <c r="I320" t="s">
         <v>23</v>
@@ -37969,14 +38012,21 @@
       </c>
       <c r="K320">
         <f>J320*G320</f>
-        <v>0.23680000000000001</v>
+        <v>22.429507495117189</v>
       </c>
       <c r="M320" t="s">
         <v>24</v>
       </c>
       <c r="N320">
-        <f>(K320/12) * 1000</f>
-        <v>19.733333333333334</v>
+        <f>K320*S320</f>
+        <v>6.230417004126414</v>
+      </c>
+      <c r="Q320" t="s">
+        <v>26</v>
+      </c>
+      <c r="S320">
+        <f>0.2777777</f>
+        <v>0.27777770000000002</v>
       </c>
     </row>
     <row r="321" spans="4:15" x14ac:dyDescent="0.3">
@@ -37984,16 +38034,16 @@
         <v>16</v>
       </c>
       <c r="G321">
-        <f>G320+I310</f>
-        <v>6.4600000000000005E-2</v>
+        <f>G320+I315</f>
+        <v>6.2394590942382813</v>
       </c>
       <c r="K321">
         <f>G321*J320</f>
-        <v>0.23902000000000004</v>
+        <v>23.085998648681642</v>
       </c>
       <c r="N321">
-        <f>(K321/12) * 1000</f>
-        <v>19.918333333333337</v>
+        <f>K321*S320</f>
+        <v>6.412775606833895</v>
       </c>
     </row>
     <row r="322" spans="4:15" x14ac:dyDescent="0.3">
@@ -38001,16 +38051,16 @@
         <v>17</v>
       </c>
       <c r="G322">
-        <f>G320+I311</f>
-        <v>6.4001299999999997E-2</v>
+        <f>G320+I316</f>
+        <v>6.0624134844909667</v>
       </c>
       <c r="K322">
         <f>G322*J320</f>
-        <v>0.23680481</v>
+        <v>22.430929892616579</v>
       </c>
       <c r="N322">
-        <f>(K322/12) * 1000</f>
-        <v>19.733734166666665</v>
+        <f>K322*S320</f>
+        <v>6.2308121144322808</v>
       </c>
     </row>
     <row r="323" spans="4:15" x14ac:dyDescent="0.3">
@@ -38018,16 +38068,16 @@
         <v>18</v>
       </c>
       <c r="G323">
-        <f>G320+I312</f>
-        <v>6.4000399999999999E-2</v>
+        <f>G320+I317</f>
+        <v>6.0621473394287113</v>
       </c>
       <c r="K323">
         <f>G323*J320</f>
-        <v>0.23680148000000001</v>
+        <v>22.429945155886234</v>
       </c>
       <c r="N323">
-        <f>(K323/12) * 1000</f>
-        <v>19.733456666666665</v>
+        <f>K323*S320</f>
+        <v>6.23053857652822</v>
       </c>
     </row>
     <row r="327" spans="4:15" x14ac:dyDescent="0.3">
@@ -38185,10 +38235,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:O338"/>
+  <dimension ref="A1:S338"/>
   <sheetViews>
     <sheetView topLeftCell="A298" workbookViewId="0">
-      <selection activeCell="H309" sqref="H309:L312"/>
+      <selection activeCell="K319" sqref="K319:N319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -50253,7 +50303,7 @@
         <v>298.47171020507813</v>
       </c>
     </row>
-    <row r="306" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="306" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D306" t="s">
         <v>9</v>
       </c>
@@ -50262,7 +50312,7 @@
         <v>295.72354125976563</v>
       </c>
     </row>
-    <row r="308" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="308" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D308" t="s">
         <v>10</v>
       </c>
@@ -50282,7 +50332,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="309" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H309">
         <f>20*10^-3</f>
         <v>0.02</v>
@@ -50296,7 +50346,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="310" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="310" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E310" t="s">
         <v>16</v>
       </c>
@@ -50305,7 +50355,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="311" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="311" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E311" t="s">
         <v>17</v>
       </c>
@@ -50314,7 +50364,7 @@
         <v>1.3E-6</v>
       </c>
     </row>
-    <row r="312" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="312" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E312" t="s">
         <v>18</v>
       </c>
@@ -50323,7 +50373,7 @@
         <v>3.9999999999999998E-7</v>
       </c>
     </row>
-    <row r="314" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="314" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D314" t="s">
         <v>19</v>
       </c>
@@ -50340,25 +50390,33 @@
         <v>5.9694342041015629</v>
       </c>
     </row>
-    <row r="315" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="315" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I315">
         <f>I306*I310</f>
         <v>0.17743412475585935</v>
       </c>
     </row>
-    <row r="316" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="316" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I316">
         <f>I306*I311</f>
         <v>3.8444060363769533E-4</v>
       </c>
     </row>
-    <row r="317" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="317" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I317">
         <f>I306*I312</f>
         <v>1.1828941650390624E-4</v>
       </c>
     </row>
-    <row r="320" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="319" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="K319" t="s">
+        <v>27</v>
+      </c>
+      <c r="N319" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="320" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D320" t="s">
         <v>20</v>
       </c>
@@ -50366,8 +50424,8 @@
         <v>21</v>
       </c>
       <c r="G320">
-        <f>H309+K309+L309</f>
-        <v>6.4000000000000001E-2</v>
+        <f>H314+K314+L314</f>
+        <v>6.0618806152343758</v>
       </c>
       <c r="I320" t="s">
         <v>23</v>
@@ -50377,14 +50435,21 @@
       </c>
       <c r="K320">
         <f>J320*G320</f>
-        <v>0.23680000000000001</v>
+        <v>22.42895827636719</v>
       </c>
       <c r="M320" t="s">
         <v>24</v>
       </c>
       <c r="N320">
-        <f>(K320/12) * 1000</f>
-        <v>19.733333333333334</v>
+        <f>K320*S320</f>
+        <v>6.2302644434052432</v>
+      </c>
+      <c r="Q320" t="s">
+        <v>26</v>
+      </c>
+      <c r="S320">
+        <f>0.2777777</f>
+        <v>0.27777770000000002</v>
       </c>
     </row>
     <row r="321" spans="4:15" x14ac:dyDescent="0.3">
@@ -50392,16 +50457,16 @@
         <v>16</v>
       </c>
       <c r="G321">
-        <f>G320+I310</f>
-        <v>6.4600000000000005E-2</v>
+        <f>G320+I315</f>
+        <v>6.2393147399902356</v>
       </c>
       <c r="K321">
         <f>G321*J320</f>
-        <v>0.23902000000000004</v>
+        <v>23.085464537963873</v>
       </c>
       <c r="N321">
-        <f>(K321/12) * 1000</f>
-        <v>19.918333333333337</v>
+        <f>K321*S320</f>
+        <v>6.4126272427871678</v>
       </c>
     </row>
     <row r="322" spans="4:15" x14ac:dyDescent="0.3">
@@ -50409,16 +50474,16 @@
         <v>17</v>
       </c>
       <c r="G322">
-        <f>G320+I311</f>
-        <v>6.4001299999999997E-2</v>
+        <f>G320+I316</f>
+        <v>6.0622650558380133</v>
       </c>
       <c r="K322">
         <f>G322*J320</f>
-        <v>0.23680481</v>
+        <v>22.430380706600651</v>
       </c>
       <c r="N322">
-        <f>(K322/12) * 1000</f>
-        <v>19.733734166666665</v>
+        <f>K322*S320</f>
+        <v>6.2306595628039041</v>
       </c>
     </row>
     <row r="323" spans="4:15" x14ac:dyDescent="0.3">
@@ -50426,16 +50491,16 @@
         <v>18</v>
       </c>
       <c r="G323">
-        <f>G320+I312</f>
-        <v>6.4000399999999999E-2</v>
+        <f>G320+I317</f>
+        <v>6.0619989046508795</v>
       </c>
       <c r="K323">
         <f>G323*J320</f>
-        <v>0.23680148000000001</v>
+        <v>22.429395947208256</v>
       </c>
       <c r="N323">
-        <f>(K323/12) * 1000</f>
-        <v>19.733456666666665</v>
+        <f>K323*S320</f>
+        <v>6.2303860186048308</v>
       </c>
     </row>
     <row r="327" spans="4:15" x14ac:dyDescent="0.3">
@@ -50593,10 +50658,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:O338"/>
+  <dimension ref="A1:S338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E298" workbookViewId="0">
-      <selection activeCell="L309" sqref="L309"/>
+    <sheetView tabSelected="1" topLeftCell="G298" workbookViewId="0">
+      <selection activeCell="K319" sqref="K319:N319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -62666,7 +62731,7 @@
         <v>298.4716796875</v>
       </c>
     </row>
-    <row r="306" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="306" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D306" t="s">
         <v>9</v>
       </c>
@@ -62675,7 +62740,7 @@
         <v>295.72064208984375</v>
       </c>
     </row>
-    <row r="308" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="308" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D308" t="s">
         <v>10</v>
       </c>
@@ -62695,7 +62760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="309" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H309">
         <f>20*10^-3</f>
         <v>0.02</v>
@@ -62709,7 +62774,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="310" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="310" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E310" t="s">
         <v>16</v>
       </c>
@@ -62718,7 +62783,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="311" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="311" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E311" t="s">
         <v>17</v>
       </c>
@@ -62727,7 +62792,7 @@
         <v>1.3E-6</v>
       </c>
     </row>
-    <row r="312" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="312" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E312" t="s">
         <v>18</v>
       </c>
@@ -62736,7 +62801,7 @@
         <v>3.9999999999999998E-7</v>
       </c>
     </row>
-    <row r="314" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="314" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D314" t="s">
         <v>19</v>
       </c>
@@ -62756,25 +62821,33 @@
         <v>5.9694335937499998</v>
       </c>
     </row>
-    <row r="315" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="315" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I315">
         <f>I306*I310</f>
         <v>0.17743238525390623</v>
       </c>
     </row>
-    <row r="316" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="316" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I316">
         <f>I306*I311</f>
         <v>3.8443683471679687E-4</v>
       </c>
     </row>
-    <row r="317" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="317" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I317">
         <f>I306*I312</f>
         <v>1.1828825683593749E-4</v>
       </c>
     </row>
-    <row r="320" spans="4:14" x14ac:dyDescent="0.3">
+    <row r="319" spans="4:19" x14ac:dyDescent="0.3">
+      <c r="K319" t="s">
+        <v>27</v>
+      </c>
+      <c r="N319" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="320" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D320" t="s">
         <v>20</v>
       </c>
@@ -62782,8 +62855,8 @@
         <v>21</v>
       </c>
       <c r="G320">
-        <f>H309+K309+L309</f>
-        <v>6.4000000000000001E-2</v>
+        <f>H314+K314+L314</f>
+        <v>6.061950927734375</v>
       </c>
       <c r="I320" t="s">
         <v>23</v>
@@ -62793,14 +62866,21 @@
       </c>
       <c r="K320">
         <f>J320*G320</f>
-        <v>0.23680000000000001</v>
+        <v>22.429218432617187</v>
       </c>
       <c r="M320" t="s">
         <v>24</v>
       </c>
       <c r="N320">
-        <f>(K320/12) * 1000</f>
-        <v>19.733333333333334</v>
+        <f>K320*S320</f>
+        <v>6.2303367090100075</v>
+      </c>
+      <c r="Q320" t="s">
+        <v>26</v>
+      </c>
+      <c r="S320">
+        <f>0.2777777</f>
+        <v>0.27777770000000002</v>
       </c>
     </row>
     <row r="321" spans="4:15" x14ac:dyDescent="0.3">
@@ -62808,16 +62888,16 @@
         <v>16</v>
       </c>
       <c r="G321">
-        <f>G320+I310</f>
-        <v>6.4600000000000005E-2</v>
+        <f>G320+I315</f>
+        <v>6.2393833129882816</v>
       </c>
       <c r="K321">
         <f>G321*J320</f>
-        <v>0.23902000000000004</v>
+        <v>23.085718258056644</v>
       </c>
       <c r="N321">
-        <f>(K321/12) * 1000</f>
-        <v>19.918333333333337</v>
+        <f>K321*S320</f>
+        <v>6.4126977205709812</v>
       </c>
     </row>
     <row r="322" spans="4:15" x14ac:dyDescent="0.3">
@@ -62825,16 +62905,16 @@
         <v>17</v>
       </c>
       <c r="G322">
-        <f>G320+I311</f>
-        <v>6.4001299999999997E-2</v>
+        <f>G320+I316</f>
+        <v>6.0623353645690923</v>
       </c>
       <c r="K322">
         <f>G322*J320</f>
-        <v>0.23680481</v>
+        <v>22.430640848905643</v>
       </c>
       <c r="N322">
-        <f>(K322/12) * 1000</f>
-        <v>19.733734166666665</v>
+        <f>K322*S320</f>
+        <v>6.2307318245350576</v>
       </c>
     </row>
     <row r="323" spans="4:15" x14ac:dyDescent="0.3">
@@ -62842,16 +62922,16 @@
         <v>18</v>
       </c>
       <c r="G323">
-        <f>G320+I312</f>
-        <v>6.4000399999999999E-2</v>
+        <f>G320+I317</f>
+        <v>6.0620692159912108</v>
       </c>
       <c r="K323">
         <f>G323*J320</f>
-        <v>0.23680148000000001</v>
+        <v>22.429656099167481</v>
       </c>
       <c r="N323">
-        <f>(K323/12) * 1000</f>
-        <v>19.733456666666665</v>
+        <f>K323*S320</f>
+        <v>6.2304582830177155</v>
       </c>
     </row>
     <row r="327" spans="4:15" x14ac:dyDescent="0.3">

</xml_diff>